<commit_message>
fix the po details form
</commit_message>
<xml_diff>
--- a/docs/PO Mgmt - For New Tool_Pardeep.xlsx
+++ b/docs/PO Mgmt - For New Tool_Pardeep.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PO-Management\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\po-mgmt\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6930F1-BB07-45D1-97FC-B41FB0398C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF31C0D7-636D-49E6-9F71-AEB726ED678E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker Updates" sheetId="1" r:id="rId1"/>
@@ -5612,11 +5612,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D31455B-CAB4-4C9E-B655-603B0297CDFA}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A2:O33"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
+      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
@@ -5729,7 +5730,7 @@
       </c>
       <c r="O3" s="24"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" hidden="1">
       <c r="A4" s="26" t="s">
         <v>41</v>
       </c>
@@ -5776,7 +5777,7 @@
       </c>
       <c r="O4" s="24"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" hidden="1">
       <c r="A5" s="26" t="s">
         <v>44</v>
       </c>
@@ -5823,7 +5824,7 @@
       </c>
       <c r="O5" s="24"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" hidden="1">
       <c r="A6" s="26" t="s">
         <v>46</v>
       </c>
@@ -5870,7 +5871,7 @@
       </c>
       <c r="O6" s="24"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" hidden="1">
       <c r="A7" s="26" t="s">
         <v>48</v>
       </c>
@@ -5917,7 +5918,7 @@
       </c>
       <c r="O7" s="24"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" hidden="1">
       <c r="A8" s="23" t="s">
         <v>50</v>
       </c>
@@ -5964,7 +5965,7 @@
       </c>
       <c r="O8" s="24"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" hidden="1">
       <c r="A9" s="23" t="s">
         <v>52</v>
       </c>
@@ -6005,7 +6006,7 @@
       </c>
       <c r="O9" s="24"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" hidden="1">
       <c r="A10" s="23" t="s">
         <v>52</v>
       </c>
@@ -6046,7 +6047,7 @@
       </c>
       <c r="O10" s="24"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" hidden="1">
       <c r="A11" s="23" t="s">
         <v>52</v>
       </c>
@@ -6087,7 +6088,7 @@
       </c>
       <c r="O11" s="24"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" hidden="1">
       <c r="A12" s="26" t="s">
         <v>53</v>
       </c>
@@ -6128,7 +6129,7 @@
       </c>
       <c r="O12" s="24"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" hidden="1">
       <c r="A13" s="26" t="s">
         <v>53</v>
       </c>
@@ -6165,7 +6166,7 @@
       </c>
       <c r="O13" s="24"/>
     </row>
-    <row r="14" spans="1:15" ht="14.4">
+    <row r="14" spans="1:15" ht="14.4" hidden="1">
       <c r="A14" s="26" t="s">
         <v>53</v>
       </c>
@@ -6200,7 +6201,7 @@
       </c>
       <c r="O14" s="24"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" hidden="1">
       <c r="A15" s="26" t="s">
         <v>113</v>
       </c>
@@ -6239,7 +6240,7 @@
       </c>
       <c r="O15" s="24"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" hidden="1">
       <c r="A16" s="26" t="s">
         <v>113</v>
       </c>
@@ -6278,7 +6279,7 @@
       </c>
       <c r="O16" s="24"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" hidden="1">
       <c r="A17" s="26"/>
       <c r="B17" s="23" t="s">
         <v>56</v>
@@ -6315,7 +6316,7 @@
       </c>
       <c r="O17" s="24"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" hidden="1">
       <c r="A18" s="26"/>
       <c r="B18" s="23" t="s">
         <v>56</v>
@@ -6350,7 +6351,7 @@
       </c>
       <c r="O18" s="24"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" hidden="1">
       <c r="A19" s="26"/>
       <c r="B19" s="23" t="s">
         <v>57</v>
@@ -6375,7 +6376,7 @@
       </c>
       <c r="O19" s="24"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" hidden="1">
       <c r="A20" s="26"/>
       <c r="B20" s="23" t="s">
         <v>58</v>
@@ -6400,7 +6401,7 @@
       </c>
       <c r="O20" s="24"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" hidden="1">
       <c r="A21" s="26" t="s">
         <v>59</v>
       </c>
@@ -6445,7 +6446,7 @@
       </c>
       <c r="O21" s="24"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" hidden="1">
       <c r="A22" s="26" t="s">
         <v>123</v>
       </c>
@@ -6490,7 +6491,7 @@
       </c>
       <c r="O22" s="24"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" hidden="1">
       <c r="A23" s="26" t="s">
         <v>63</v>
       </c>
@@ -6533,7 +6534,7 @@
       </c>
       <c r="O23" s="24"/>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" hidden="1">
       <c r="A24" s="26" t="s">
         <v>65</v>
       </c>
@@ -6576,7 +6577,7 @@
       </c>
       <c r="O24" s="24"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" hidden="1">
       <c r="A25" s="23" t="s">
         <v>52</v>
       </c>
@@ -6621,7 +6622,7 @@
       </c>
       <c r="O25" s="24"/>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" hidden="1">
       <c r="A26" s="23" t="s">
         <v>66</v>
       </c>
@@ -6668,7 +6669,7 @@
       </c>
       <c r="O26" s="24"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" hidden="1">
       <c r="A27" s="26" t="s">
         <v>69</v>
       </c>
@@ -6715,7 +6716,7 @@
       </c>
       <c r="O27" s="24"/>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" hidden="1">
       <c r="A28" s="26" t="s">
         <v>70</v>
       </c>
@@ -6760,7 +6761,7 @@
       </c>
       <c r="O28" s="24"/>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" hidden="1">
       <c r="A29" s="23" t="s">
         <v>71</v>
       </c>
@@ -6807,7 +6808,7 @@
       </c>
       <c r="O29" s="24"/>
     </row>
-    <row r="30" spans="1:15" ht="14.4">
+    <row r="30" spans="1:15" ht="14.4" hidden="1">
       <c r="A30" s="112"/>
       <c r="B30" s="112" t="s">
         <v>72</v>
@@ -6841,7 +6842,7 @@
         <v>Cinesonic Audio Visual Pvt Ltd</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="14.4">
+    <row r="31" spans="1:15" ht="14.4" hidden="1">
       <c r="A31" s="112"/>
       <c r="B31" s="112" t="s">
         <v>72</v>
@@ -6875,7 +6876,7 @@
         <v>Cinesonic Audio Visual Pvt Ltd</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="14.4">
+    <row r="32" spans="1:15" ht="14.4" hidden="1">
       <c r="A32" s="157" t="s">
         <v>73</v>
       </c>
@@ -6921,7 +6922,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="14.4">
+    <row r="33" spans="1:14" ht="14.4" hidden="1">
       <c r="A33" s="65" t="s">
         <v>75</v>
       </c>
@@ -6968,7 +6969,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:N33" xr:uid="{1D31455B-CAB4-4C9E-B655-603B0297CDFA}"/>
+  <autoFilter ref="A2:N33" xr:uid="{1D31455B-CAB4-4C9E-B655-603B0297CDFA}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="4500095281"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1" display="FC2024-243.pdf (application/pdf)  " xr:uid="{CE866A8E-EB30-4987-A223-FEBEB5CFBA6B}"/>
   </hyperlinks>
@@ -6979,12 +6986,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD95930-0488-4552-AB38-23ACBD525592}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:M219"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F37" sqref="F37"/>
-      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
+      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7013,15 +7021,15 @@
       <c r="F1" s="281"/>
       <c r="G1" s="256">
         <f>SUBTOTAL(9,G3:G1048576)</f>
-        <v>38762422.659999982</v>
+        <v>1328307.75</v>
       </c>
       <c r="H1" s="256">
         <f>SUBTOTAL(9,H3:H1048576)</f>
-        <v>775248.4532000008</v>
+        <v>26566.155000000002</v>
       </c>
       <c r="I1" s="256">
         <f>SUBTOTAL(9,I3:I1048576)</f>
-        <v>44964410.285599999</v>
+        <v>1540836.9899999998</v>
       </c>
       <c r="J1" s="255"/>
       <c r="K1" s="281"/>
@@ -7069,7 +7077,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" hidden="1">
       <c r="A3" s="260" t="s">
         <v>41</v>
       </c>
@@ -7109,7 +7117,7 @@
         <v>VRATA TECH SOLUTIONS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" hidden="1">
       <c r="A4" s="257" t="s">
         <v>41</v>
       </c>
@@ -7119,9 +7127,7 @@
       <c r="C4" s="257">
         <v>4500095281</v>
       </c>
-      <c r="D4" s="254">
-        <v>4500095281</v>
-      </c>
+      <c r="D4" s="254"/>
       <c r="E4" s="257" t="s">
         <v>156</v>
       </c>
@@ -7152,7 +7158,7 @@
         <v>VRATA TECH SOLUTIONS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" hidden="1">
       <c r="A5" s="257" t="s">
         <v>41</v>
       </c>
@@ -7193,7 +7199,7 @@
         <v>VRATA TECH SOLUTIONS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" hidden="1">
       <c r="A6" s="257" t="s">
         <v>41</v>
       </c>
@@ -7236,7 +7242,7 @@
         <v>VRATA TECH SOLUTIONS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" hidden="1">
       <c r="A7" s="257" t="s">
         <v>41</v>
       </c>
@@ -7573,7 +7579,7 @@
         <v>BCT Consulting Private Limited</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" hidden="1">
       <c r="A15" s="257" t="s">
         <v>46</v>
       </c>
@@ -7616,7 +7622,7 @@
         <v>CANTICLE TECHNOLOGIES PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" hidden="1">
       <c r="A16" s="257" t="s">
         <v>46</v>
       </c>
@@ -7659,7 +7665,7 @@
         <v>CANTICLE TECHNOLOGIES PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" hidden="1">
       <c r="A17" s="260" t="s">
         <v>48</v>
       </c>
@@ -7701,7 +7707,7 @@
         <v>TRIBAL SOLUTIONS CONSULTING SERVICES PVT</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" hidden="1">
       <c r="A18" s="257" t="s">
         <v>48</v>
       </c>
@@ -7743,7 +7749,7 @@
         <v>TRIBAL SOLUTIONS CONSULTING SERVICES PVT</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" hidden="1">
       <c r="A19" s="257" t="s">
         <v>48</v>
       </c>
@@ -7785,7 +7791,7 @@
         <v>TRIBAL SOLUTIONS CONSULTING SERVICES PVT</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" hidden="1">
       <c r="A20" s="257" t="s">
         <v>48</v>
       </c>
@@ -7827,7 +7833,7 @@
         <v>TRIBAL SOLUTIONS CONSULTING SERVICES PVT</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" hidden="1">
       <c r="A21" s="255" t="s">
         <v>48</v>
       </c>
@@ -7869,7 +7875,7 @@
         <v>TRIBAL SOLUTIONS CONSULTING SERVICES PVT</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" hidden="1">
       <c r="A22" s="101" t="s">
         <v>50</v>
       </c>
@@ -7912,7 +7918,7 @@
         <v>CARMATEC IT SOLUTIONS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" hidden="1">
       <c r="A23" s="101" t="s">
         <v>50</v>
       </c>
@@ -7955,7 +7961,7 @@
         <v>CARMATEC IT SOLUTIONS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" hidden="1">
       <c r="A24" s="101" t="s">
         <v>50</v>
       </c>
@@ -7998,7 +8004,7 @@
         <v>CARMATEC IT SOLUTIONS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" hidden="1">
       <c r="A25" s="101" t="s">
         <v>50</v>
       </c>
@@ -8041,7 +8047,7 @@
         <v>CARMATEC IT SOLUTIONS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" hidden="1">
       <c r="A26" s="101" t="s">
         <v>50</v>
       </c>
@@ -8084,7 +8090,7 @@
         <v>CARMATEC IT SOLUTIONS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" hidden="1">
       <c r="A27" s="101" t="s">
         <v>50</v>
       </c>
@@ -8127,7 +8133,7 @@
         <v>CARMATEC IT SOLUTIONS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" hidden="1">
       <c r="A28" s="260"/>
       <c r="B28" s="148" t="s">
         <v>189</v>
@@ -8168,7 +8174,7 @@
         <v>Winnovation Education Services Pvt</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" hidden="1">
       <c r="A29" s="257"/>
       <c r="B29" s="101" t="s">
         <v>189</v>
@@ -8209,7 +8215,7 @@
         <v>Winnovation Education Services Pvt</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" hidden="1">
       <c r="A30" s="257"/>
       <c r="B30" s="101" t="s">
         <v>189</v>
@@ -8250,7 +8256,7 @@
         <v>Winnovation Education Services Pvt</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" hidden="1">
       <c r="A31" s="257"/>
       <c r="B31" s="101" t="s">
         <v>189</v>
@@ -8284,7 +8290,7 @@
         <v>SeaInfonet Pvt Ltd</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" hidden="1">
       <c r="A32" s="257"/>
       <c r="B32" s="101" t="s">
         <v>189</v>
@@ -8318,7 +8324,7 @@
         <v>SeaInfonet Pvt Ltd</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" hidden="1">
       <c r="A33" s="257"/>
       <c r="B33" s="101" t="s">
         <v>189</v>
@@ -8352,7 +8358,7 @@
         <v>SeaInfonet Pvt Ltd</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" hidden="1">
       <c r="A34" s="257"/>
       <c r="B34" s="101" t="s">
         <v>196</v>
@@ -8390,7 +8396,7 @@
         <v>AUROPRO SOFT SYSTEMS PVT LTD</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" hidden="1">
       <c r="A35" s="257"/>
       <c r="B35" s="101" t="s">
         <v>196</v>
@@ -8428,7 +8434,7 @@
         <v>AUROPRO SOFT SYSTEMS PVT LTD</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" hidden="1">
       <c r="A36" s="257"/>
       <c r="B36" s="101" t="s">
         <v>196</v>
@@ -8469,7 +8475,7 @@
         <v>AUROPRO SOFT SYSTEMS PVT LTD</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" hidden="1">
       <c r="A37" s="257"/>
       <c r="B37" s="101" t="s">
         <v>56</v>
@@ -8507,7 +8513,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" hidden="1">
       <c r="A38" s="257"/>
       <c r="B38" s="101" t="s">
         <v>57</v>
@@ -8545,7 +8551,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" hidden="1">
       <c r="A39" s="257"/>
       <c r="B39" s="101" t="s">
         <v>57</v>
@@ -8583,7 +8589,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" hidden="1">
       <c r="A40" s="257"/>
       <c r="B40" s="101" t="s">
         <v>56</v>
@@ -8621,7 +8627,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" hidden="1">
       <c r="A41" s="257"/>
       <c r="B41" s="101" t="s">
         <v>56</v>
@@ -8659,7 +8665,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" hidden="1">
       <c r="A42" s="257"/>
       <c r="B42" s="101" t="s">
         <v>56</v>
@@ -8697,7 +8703,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" hidden="1">
       <c r="A43" s="257"/>
       <c r="B43" s="101" t="s">
         <v>57</v>
@@ -8735,7 +8741,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" hidden="1">
       <c r="A44" s="257"/>
       <c r="B44" s="101" t="s">
         <v>57</v>
@@ -8773,7 +8779,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" hidden="1">
       <c r="A45" s="257"/>
       <c r="B45" s="101" t="s">
         <v>57</v>
@@ -8811,7 +8817,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" hidden="1">
       <c r="A46" s="257"/>
       <c r="B46" s="101" t="s">
         <v>57</v>
@@ -8849,7 +8855,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" hidden="1">
       <c r="A47" s="257"/>
       <c r="B47" s="101" t="s">
         <v>57</v>
@@ -8887,7 +8893,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" hidden="1">
       <c r="A48" s="257"/>
       <c r="B48" s="101" t="s">
         <v>56</v>
@@ -8925,7 +8931,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" hidden="1">
       <c r="A49" s="257"/>
       <c r="B49" s="101" t="s">
         <v>56</v>
@@ -8963,7 +8969,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" hidden="1">
       <c r="A50" s="257"/>
       <c r="B50" s="101" t="s">
         <v>56</v>
@@ -9001,7 +9007,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" hidden="1">
       <c r="A51" s="257"/>
       <c r="B51" s="101" t="s">
         <v>57</v>
@@ -9039,7 +9045,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" hidden="1">
       <c r="A52" s="257"/>
       <c r="B52" s="101" t="s">
         <v>57</v>
@@ -9077,7 +9083,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" hidden="1">
       <c r="A53" s="257"/>
       <c r="B53" s="101" t="s">
         <v>57</v>
@@ -9115,7 +9121,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" hidden="1">
       <c r="A54" s="257"/>
       <c r="B54" s="101" t="s">
         <v>56</v>
@@ -9153,7 +9159,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" hidden="1">
       <c r="A55" s="257"/>
       <c r="B55" s="101" t="s">
         <v>56</v>
@@ -9191,7 +9197,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" hidden="1">
       <c r="A56" s="257"/>
       <c r="B56" s="101" t="s">
         <v>56</v>
@@ -9229,7 +9235,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" hidden="1">
       <c r="A57" s="257"/>
       <c r="B57" s="101" t="s">
         <v>56</v>
@@ -9267,7 +9273,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" hidden="1">
       <c r="A58" s="257"/>
       <c r="B58" s="101" t="s">
         <v>56</v>
@@ -9305,7 +9311,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" hidden="1">
       <c r="A59" s="257"/>
       <c r="B59" s="101" t="s">
         <v>58</v>
@@ -9343,7 +9349,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" hidden="1">
       <c r="A60" s="257"/>
       <c r="B60" s="101" t="s">
         <v>57</v>
@@ -9381,7 +9387,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" hidden="1">
       <c r="A61" s="257"/>
       <c r="B61" s="101" t="s">
         <v>57</v>
@@ -9419,7 +9425,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" hidden="1">
       <c r="A62" s="257"/>
       <c r="B62" s="101" t="s">
         <v>58</v>
@@ -9457,7 +9463,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" hidden="1">
       <c r="A63" s="257"/>
       <c r="B63" s="101" t="s">
         <v>58</v>
@@ -9491,7 +9497,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" hidden="1">
       <c r="A64" s="257"/>
       <c r="B64" s="101" t="s">
         <v>56</v>
@@ -9525,7 +9531,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" hidden="1">
       <c r="A65" s="257"/>
       <c r="B65" s="101" t="s">
         <v>57</v>
@@ -9559,7 +9565,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" hidden="1">
       <c r="A66" s="257"/>
       <c r="B66" s="101" t="s">
         <v>57</v>
@@ -9593,7 +9599,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" hidden="1">
       <c r="A67" s="257"/>
       <c r="B67" s="101" t="s">
         <v>57</v>
@@ -9627,7 +9633,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" hidden="1">
       <c r="A68" s="257"/>
       <c r="B68" s="101" t="s">
         <v>56</v>
@@ -9665,7 +9671,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" hidden="1">
       <c r="A69" s="257"/>
       <c r="B69" s="101" t="s">
         <v>56</v>
@@ -9703,7 +9709,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" hidden="1">
       <c r="A70" s="257"/>
       <c r="B70" s="101" t="s">
         <v>56</v>
@@ -9741,7 +9747,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" hidden="1">
       <c r="A71" s="257"/>
       <c r="B71" s="101" t="s">
         <v>56</v>
@@ -9779,7 +9785,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" hidden="1">
       <c r="A72" s="257"/>
       <c r="B72" s="101" t="s">
         <v>57</v>
@@ -9820,7 +9826,7 @@
         <v>BUSYBOTS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" hidden="1">
       <c r="A73" s="257"/>
       <c r="B73" s="101" t="s">
         <v>236</v>
@@ -9858,7 +9864,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:13" hidden="1">
       <c r="A74" s="257"/>
       <c r="B74" s="101" t="s">
         <v>236</v>
@@ -9896,7 +9902,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" spans="1:13" hidden="1">
       <c r="A75" s="257"/>
       <c r="B75" s="101" t="s">
         <v>236</v>
@@ -9934,7 +9940,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" hidden="1">
       <c r="A76" s="257"/>
       <c r="B76" s="101" t="s">
         <v>236</v>
@@ -9972,7 +9978,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" hidden="1">
       <c r="A77" s="257"/>
       <c r="B77" s="101" t="s">
         <v>236</v>
@@ -10010,7 +10016,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" hidden="1">
       <c r="A78" s="257"/>
       <c r="B78" s="101" t="s">
         <v>236</v>
@@ -10048,7 +10054,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" hidden="1">
       <c r="A79" s="257"/>
       <c r="B79" s="101" t="s">
         <v>236</v>
@@ -10086,7 +10092,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:13" hidden="1">
       <c r="A80" s="257"/>
       <c r="B80" s="101" t="s">
         <v>236</v>
@@ -10124,7 +10130,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" hidden="1">
       <c r="A81" s="257"/>
       <c r="B81" s="101" t="s">
         <v>236</v>
@@ -10162,7 +10168,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="82" spans="1:13">
+    <row r="82" spans="1:13" hidden="1">
       <c r="A82" s="257"/>
       <c r="B82" s="101" t="s">
         <v>236</v>
@@ -10200,7 +10206,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:13" hidden="1">
       <c r="A83" s="257"/>
       <c r="B83" s="101" t="s">
         <v>247</v>
@@ -10238,7 +10244,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:13" hidden="1">
       <c r="A84" s="257"/>
       <c r="B84" s="101" t="s">
         <v>247</v>
@@ -10276,7 +10282,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" hidden="1">
       <c r="A85" s="257"/>
       <c r="B85" s="101" t="s">
         <v>247</v>
@@ -10314,7 +10320,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" hidden="1">
       <c r="A86" s="257"/>
       <c r="B86" s="101" t="s">
         <v>247</v>
@@ -10352,7 +10358,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" hidden="1">
       <c r="A87" s="257"/>
       <c r="B87" s="101" t="s">
         <v>247</v>
@@ -10390,7 +10396,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:13" hidden="1">
       <c r="A88" s="257"/>
       <c r="B88" s="101" t="s">
         <v>74</v>
@@ -10428,7 +10434,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:13" hidden="1">
       <c r="A89" s="257"/>
       <c r="B89" s="101" t="s">
         <v>74</v>
@@ -10466,7 +10472,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" hidden="1">
       <c r="A90" s="257"/>
       <c r="B90" s="101" t="s">
         <v>74</v>
@@ -10504,7 +10510,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:13" hidden="1">
       <c r="A91" s="257"/>
       <c r="B91" s="101" t="s">
         <v>74</v>
@@ -10542,7 +10548,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" hidden="1">
       <c r="A92" s="257"/>
       <c r="B92" s="101" t="s">
         <v>74</v>
@@ -10580,7 +10586,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" hidden="1">
       <c r="A93" s="257"/>
       <c r="B93" s="101" t="s">
         <v>74</v>
@@ -10618,7 +10624,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:13" hidden="1">
       <c r="A94" s="257"/>
       <c r="B94" s="101" t="s">
         <v>74</v>
@@ -10656,7 +10662,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:13" hidden="1">
       <c r="A95" s="257"/>
       <c r="B95" s="101" t="s">
         <v>74</v>
@@ -10694,7 +10700,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:13" hidden="1">
       <c r="A96" s="257"/>
       <c r="B96" s="101" t="s">
         <v>74</v>
@@ -10732,7 +10738,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="97" spans="1:13">
+    <row r="97" spans="1:13" hidden="1">
       <c r="A97" s="257"/>
       <c r="B97" s="101" t="s">
         <v>74</v>
@@ -10770,7 +10776,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:13" hidden="1">
       <c r="A98" s="257"/>
       <c r="B98" s="101" t="s">
         <v>74</v>
@@ -10808,7 +10814,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="99" spans="1:13">
+    <row r="99" spans="1:13" hidden="1">
       <c r="A99" s="257"/>
       <c r="B99" s="101" t="s">
         <v>74</v>
@@ -10846,7 +10852,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="100" spans="1:13">
+    <row r="100" spans="1:13" hidden="1">
       <c r="A100" s="257"/>
       <c r="B100" s="101" t="s">
         <v>74</v>
@@ -10884,7 +10890,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:13" hidden="1">
       <c r="A101" s="257"/>
       <c r="B101" s="101" t="s">
         <v>74</v>
@@ -10920,7 +10926,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:13" hidden="1">
       <c r="A102" s="257"/>
       <c r="B102" s="101" t="s">
         <v>74</v>
@@ -10958,7 +10964,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="103" spans="1:13">
+    <row r="103" spans="1:13" hidden="1">
       <c r="A103" s="257"/>
       <c r="B103" s="101" t="s">
         <v>74</v>
@@ -10996,7 +11002,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="104" spans="1:13">
+    <row r="104" spans="1:13" hidden="1">
       <c r="A104" s="257"/>
       <c r="B104" s="101" t="s">
         <v>74</v>
@@ -11034,7 +11040,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="105" spans="1:13">
+    <row r="105" spans="1:13" hidden="1">
       <c r="A105" s="257"/>
       <c r="B105" s="101" t="s">
         <v>74</v>
@@ -11072,7 +11078,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="106" spans="1:13">
+    <row r="106" spans="1:13" hidden="1">
       <c r="A106" s="257"/>
       <c r="B106" s="101" t="s">
         <v>74</v>
@@ -11110,7 +11116,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="107" spans="1:13">
+    <row r="107" spans="1:13" hidden="1">
       <c r="A107" s="257"/>
       <c r="B107" s="101" t="s">
         <v>74</v>
@@ -11148,7 +11154,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="108" spans="1:13">
+    <row r="108" spans="1:13" hidden="1">
       <c r="A108" s="257"/>
       <c r="B108" s="101" t="s">
         <v>74</v>
@@ -11186,7 +11192,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="109" spans="1:13">
+    <row r="109" spans="1:13" hidden="1">
       <c r="A109" s="257"/>
       <c r="B109" s="101" t="s">
         <v>74</v>
@@ -11224,7 +11230,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="110" spans="1:13" s="57" customFormat="1">
+    <row r="110" spans="1:13" s="57" customFormat="1" hidden="1">
       <c r="A110" s="116"/>
       <c r="B110" s="116" t="s">
         <v>74</v>
@@ -11249,7 +11255,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="111" spans="1:13" s="57" customFormat="1">
+    <row r="111" spans="1:13" s="57" customFormat="1" hidden="1">
       <c r="A111" s="116"/>
       <c r="B111" s="116" t="s">
         <v>74</v>
@@ -11287,7 +11293,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="112" spans="1:13">
+    <row r="112" spans="1:13" hidden="1">
       <c r="A112" s="257"/>
       <c r="B112" s="101" t="s">
         <v>74</v>
@@ -11325,7 +11331,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="113" spans="1:13">
+    <row r="113" spans="1:13" hidden="1">
       <c r="A113" s="257"/>
       <c r="B113" s="101" t="s">
         <v>74</v>
@@ -11363,7 +11369,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="114" spans="1:13">
+    <row r="114" spans="1:13" hidden="1">
       <c r="A114" s="257"/>
       <c r="B114" s="101" t="s">
         <v>74</v>
@@ -11399,7 +11405,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="115" spans="1:13">
+    <row r="115" spans="1:13" hidden="1">
       <c r="A115" s="257"/>
       <c r="B115" s="101" t="s">
         <v>74</v>
@@ -11435,7 +11441,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="116" spans="1:13">
+    <row r="116" spans="1:13" hidden="1">
       <c r="A116" s="257"/>
       <c r="B116" s="101" t="s">
         <v>74</v>
@@ -11471,7 +11477,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="117" spans="1:13">
+    <row r="117" spans="1:13" hidden="1">
       <c r="A117" s="257"/>
       <c r="B117" s="101" t="s">
         <v>74</v>
@@ -11507,7 +11513,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="118" spans="1:13">
+    <row r="118" spans="1:13" hidden="1">
       <c r="A118" s="257"/>
       <c r="B118" s="101" t="s">
         <v>74</v>
@@ -11543,7 +11549,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="119" spans="1:13">
+    <row r="119" spans="1:13" hidden="1">
       <c r="A119" s="257"/>
       <c r="B119" s="101" t="s">
         <v>74</v>
@@ -11579,7 +11585,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="120" spans="1:13">
+    <row r="120" spans="1:13" hidden="1">
       <c r="A120" s="257"/>
       <c r="B120" s="101" t="s">
         <v>74</v>
@@ -11615,7 +11621,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="121" spans="1:13">
+    <row r="121" spans="1:13" hidden="1">
       <c r="A121" s="257"/>
       <c r="B121" s="101" t="s">
         <v>74</v>
@@ -11651,7 +11657,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="122" spans="1:13">
+    <row r="122" spans="1:13" hidden="1">
       <c r="A122" s="257"/>
       <c r="B122" s="101" t="s">
         <v>74</v>
@@ -11687,7 +11693,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="123" spans="1:13">
+    <row r="123" spans="1:13" hidden="1">
       <c r="A123" s="257"/>
       <c r="B123" s="101" t="s">
         <v>74</v>
@@ -11723,7 +11729,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="124" spans="1:13">
+    <row r="124" spans="1:13" hidden="1">
       <c r="A124" s="257"/>
       <c r="B124" s="101" t="s">
         <v>74</v>
@@ -11759,7 +11765,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="125" spans="1:13">
+    <row r="125" spans="1:13" hidden="1">
       <c r="A125" s="257"/>
       <c r="B125" s="101" t="s">
         <v>74</v>
@@ -11795,7 +11801,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="126" spans="1:13">
+    <row r="126" spans="1:13" hidden="1">
       <c r="A126" s="257"/>
       <c r="B126" s="101" t="s">
         <v>74</v>
@@ -11831,7 +11837,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="127" spans="1:13">
+    <row r="127" spans="1:13" hidden="1">
       <c r="A127" s="257"/>
       <c r="B127" s="101" t="s">
         <v>74</v>
@@ -11867,7 +11873,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="128" spans="1:13">
+    <row r="128" spans="1:13" hidden="1">
       <c r="A128" s="257"/>
       <c r="B128" s="101" t="s">
         <v>74</v>
@@ -11903,7 +11909,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="129" spans="1:13">
+    <row r="129" spans="1:13" hidden="1">
       <c r="A129" s="257"/>
       <c r="B129" s="101" t="s">
         <v>74</v>
@@ -11939,7 +11945,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="130" spans="1:13">
+    <row r="130" spans="1:13" hidden="1">
       <c r="A130" s="257"/>
       <c r="B130" s="101" t="s">
         <v>74</v>
@@ -11974,7 +11980,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="131" spans="1:13">
+    <row r="131" spans="1:13" hidden="1">
       <c r="A131" s="257"/>
       <c r="B131" s="101" t="s">
         <v>74</v>
@@ -12010,7 +12016,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="132" spans="1:13">
+    <row r="132" spans="1:13" hidden="1">
       <c r="A132" s="257"/>
       <c r="B132" s="101" t="s">
         <v>74</v>
@@ -12046,7 +12052,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="133" spans="1:13">
+    <row r="133" spans="1:13" hidden="1">
       <c r="A133" s="257"/>
       <c r="B133" s="101" t="s">
         <v>74</v>
@@ -12082,7 +12088,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="134" spans="1:13">
+    <row r="134" spans="1:13" hidden="1">
       <c r="A134" s="257"/>
       <c r="B134" s="101" t="s">
         <v>74</v>
@@ -12118,7 +12124,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="135" spans="1:13">
+    <row r="135" spans="1:13" hidden="1">
       <c r="A135" s="257"/>
       <c r="B135" s="101" t="s">
         <v>74</v>
@@ -12154,7 +12160,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="136" spans="1:13">
+    <row r="136" spans="1:13" hidden="1">
       <c r="A136" s="257"/>
       <c r="B136" s="101" t="s">
         <v>74</v>
@@ -12190,7 +12196,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="137" spans="1:13">
+    <row r="137" spans="1:13" hidden="1">
       <c r="A137" s="257"/>
       <c r="B137" s="101" t="s">
         <v>74</v>
@@ -12225,7 +12231,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="138" spans="1:13">
+    <row r="138" spans="1:13" hidden="1">
       <c r="A138" s="257"/>
       <c r="B138" s="101" t="s">
         <v>74</v>
@@ -12261,7 +12267,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="139" spans="1:13">
+    <row r="139" spans="1:13" hidden="1">
       <c r="A139" s="257"/>
       <c r="B139" s="101" t="s">
         <v>74</v>
@@ -12297,7 +12303,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="140" spans="1:13">
+    <row r="140" spans="1:13" hidden="1">
       <c r="A140" s="257"/>
       <c r="B140" s="101" t="s">
         <v>74</v>
@@ -12332,7 +12338,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="141" spans="1:13">
+    <row r="141" spans="1:13" hidden="1">
       <c r="A141" s="257"/>
       <c r="B141" s="101" t="s">
         <v>74</v>
@@ -12368,7 +12374,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="142" spans="1:13">
+    <row r="142" spans="1:13" hidden="1">
       <c r="A142" s="257"/>
       <c r="B142" s="101" t="s">
         <v>74</v>
@@ -12404,7 +12410,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="143" spans="1:13">
+    <row r="143" spans="1:13" hidden="1">
       <c r="A143" s="257"/>
       <c r="B143" s="101" t="s">
         <v>74</v>
@@ -12440,7 +12446,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="144" spans="1:13">
+    <row r="144" spans="1:13" hidden="1">
       <c r="A144" s="257"/>
       <c r="B144" s="101" t="s">
         <v>74</v>
@@ -12476,7 +12482,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="145" spans="1:13">
+    <row r="145" spans="1:13" hidden="1">
       <c r="A145" s="257"/>
       <c r="B145" s="101" t="s">
         <v>74</v>
@@ -12512,7 +12518,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="146" spans="1:13">
+    <row r="146" spans="1:13" hidden="1">
       <c r="A146" s="257"/>
       <c r="B146" s="101" t="s">
         <v>74</v>
@@ -12547,7 +12553,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="147" spans="1:13">
+    <row r="147" spans="1:13" hidden="1">
       <c r="A147" s="257"/>
       <c r="B147" s="101" t="s">
         <v>74</v>
@@ -12583,7 +12589,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="148" spans="1:13">
+    <row r="148" spans="1:13" hidden="1">
       <c r="A148" s="257"/>
       <c r="B148" s="101" t="s">
         <v>74</v>
@@ -12619,7 +12625,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="149" spans="1:13">
+    <row r="149" spans="1:13" hidden="1">
       <c r="A149" s="257"/>
       <c r="B149" s="101" t="s">
         <v>74</v>
@@ -12655,7 +12661,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="150" spans="1:13">
+    <row r="150" spans="1:13" hidden="1">
       <c r="A150" s="257"/>
       <c r="B150" s="101" t="s">
         <v>74</v>
@@ -12691,7 +12697,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="151" spans="1:13">
+    <row r="151" spans="1:13" hidden="1">
       <c r="A151" s="257"/>
       <c r="B151" s="101" t="s">
         <v>74</v>
@@ -12726,7 +12732,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="152" spans="1:13">
+    <row r="152" spans="1:13" hidden="1">
       <c r="A152" s="257"/>
       <c r="B152" s="101" t="s">
         <v>74</v>
@@ -12761,7 +12767,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="153" spans="1:13">
+    <row r="153" spans="1:13" hidden="1">
       <c r="A153" s="257"/>
       <c r="B153" s="101" t="s">
         <v>74</v>
@@ -12797,7 +12803,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="154" spans="1:13">
+    <row r="154" spans="1:13" hidden="1">
       <c r="A154" s="257"/>
       <c r="B154" s="101" t="s">
         <v>74</v>
@@ -12833,7 +12839,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="155" spans="1:13">
+    <row r="155" spans="1:13" hidden="1">
       <c r="A155" s="257"/>
       <c r="B155" s="101" t="s">
         <v>74</v>
@@ -12869,7 +12875,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="156" spans="1:13">
+    <row r="156" spans="1:13" hidden="1">
       <c r="A156" s="257"/>
       <c r="B156" s="101" t="s">
         <v>74</v>
@@ -12905,7 +12911,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="157" spans="1:13">
+    <row r="157" spans="1:13" hidden="1">
       <c r="A157" s="257"/>
       <c r="B157" s="101" t="s">
         <v>74</v>
@@ -12941,7 +12947,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="158" spans="1:13">
+    <row r="158" spans="1:13" hidden="1">
       <c r="A158" s="257"/>
       <c r="B158" s="101" t="s">
         <v>74</v>
@@ -12977,7 +12983,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="159" spans="1:13">
+    <row r="159" spans="1:13" hidden="1">
       <c r="A159" s="257"/>
       <c r="B159" s="101" t="s">
         <v>74</v>
@@ -13013,7 +13019,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="160" spans="1:13">
+    <row r="160" spans="1:13" hidden="1">
       <c r="A160" s="257"/>
       <c r="B160" s="101" t="s">
         <v>74</v>
@@ -13048,7 +13054,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="161" spans="1:13">
+    <row r="161" spans="1:13" hidden="1">
       <c r="A161" s="257"/>
       <c r="B161" s="101" t="s">
         <v>74</v>
@@ -13084,7 +13090,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="162" spans="1:13">
+    <row r="162" spans="1:13" hidden="1">
       <c r="A162" s="257"/>
       <c r="B162" s="101" t="s">
         <v>74</v>
@@ -13120,7 +13126,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="163" spans="1:13">
+    <row r="163" spans="1:13" hidden="1">
       <c r="A163" s="257"/>
       <c r="B163" s="101" t="s">
         <v>74</v>
@@ -13155,7 +13161,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="164" spans="1:13">
+    <row r="164" spans="1:13" hidden="1">
       <c r="A164" s="257"/>
       <c r="B164" s="101" t="s">
         <v>74</v>
@@ -13191,7 +13197,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="165" spans="1:13">
+    <row r="165" spans="1:13" hidden="1">
       <c r="A165" s="257"/>
       <c r="B165" s="101" t="s">
         <v>74</v>
@@ -13227,7 +13233,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="166" spans="1:13">
+    <row r="166" spans="1:13" hidden="1">
       <c r="A166" s="257"/>
       <c r="B166" s="101" t="s">
         <v>74</v>
@@ -13263,7 +13269,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="167" spans="1:13">
+    <row r="167" spans="1:13" hidden="1">
       <c r="A167" s="257"/>
       <c r="B167" s="101" t="s">
         <v>74</v>
@@ -13299,7 +13305,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="168" spans="1:13">
+    <row r="168" spans="1:13" hidden="1">
       <c r="A168" s="257"/>
       <c r="B168" s="101" t="s">
         <v>74</v>
@@ -13335,7 +13341,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="169" spans="1:13">
+    <row r="169" spans="1:13" hidden="1">
       <c r="A169" s="257"/>
       <c r="B169" s="101" t="s">
         <v>74</v>
@@ -13371,7 +13377,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="170" spans="1:13">
+    <row r="170" spans="1:13" hidden="1">
       <c r="A170" s="257"/>
       <c r="B170" s="101" t="s">
         <v>74</v>
@@ -13407,7 +13413,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="171" spans="1:13">
+    <row r="171" spans="1:13" hidden="1">
       <c r="A171" s="257"/>
       <c r="B171" s="101" t="s">
         <v>74</v>
@@ -13443,7 +13449,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="172" spans="1:13">
+    <row r="172" spans="1:13" hidden="1">
       <c r="A172" s="257"/>
       <c r="B172" s="101" t="s">
         <v>74</v>
@@ -13479,7 +13485,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="173" spans="1:13">
+    <row r="173" spans="1:13" hidden="1">
       <c r="A173" s="257"/>
       <c r="B173" s="101" t="s">
         <v>74</v>
@@ -13515,7 +13521,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="174" spans="1:13">
+    <row r="174" spans="1:13" hidden="1">
       <c r="A174" s="257"/>
       <c r="B174" s="101" t="s">
         <v>74</v>
@@ -13551,7 +13557,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="175" spans="1:13">
+    <row r="175" spans="1:13" hidden="1">
       <c r="A175" s="257"/>
       <c r="B175" s="101" t="s">
         <v>74</v>
@@ -13587,7 +13593,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="176" spans="1:13">
+    <row r="176" spans="1:13" hidden="1">
       <c r="A176" s="257"/>
       <c r="B176" s="101" t="s">
         <v>74</v>
@@ -13623,7 +13629,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="177" spans="1:13">
+    <row r="177" spans="1:13" hidden="1">
       <c r="A177" s="257"/>
       <c r="B177" s="101" t="s">
         <v>74</v>
@@ -13659,7 +13665,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="178" spans="1:13">
+    <row r="178" spans="1:13" hidden="1">
       <c r="A178" s="257"/>
       <c r="B178" s="101" t="s">
         <v>74</v>
@@ -13695,7 +13701,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="179" spans="1:13">
+    <row r="179" spans="1:13" hidden="1">
       <c r="A179" s="257"/>
       <c r="B179" s="101" t="s">
         <v>74</v>
@@ -13731,7 +13737,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="180" spans="1:13">
+    <row r="180" spans="1:13" hidden="1">
       <c r="A180" s="257"/>
       <c r="B180" s="101" t="s">
         <v>74</v>
@@ -13767,7 +13773,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="181" spans="1:13">
+    <row r="181" spans="1:13" hidden="1">
       <c r="A181" s="257"/>
       <c r="B181" s="101" t="s">
         <v>74</v>
@@ -13803,7 +13809,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="182" spans="1:13">
+    <row r="182" spans="1:13" hidden="1">
       <c r="A182" s="257"/>
       <c r="B182" s="101" t="s">
         <v>74</v>
@@ -13843,7 +13849,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="183" spans="1:13">
+    <row r="183" spans="1:13" hidden="1">
       <c r="A183" s="257"/>
       <c r="B183" s="101" t="s">
         <v>74</v>
@@ -13883,7 +13889,7 @@
         <v>KAPARTHI CONSULTANCY SERVICES</v>
       </c>
     </row>
-    <row r="184" spans="1:13">
+    <row r="184" spans="1:13" hidden="1">
       <c r="A184" s="257"/>
       <c r="B184" s="101" t="s">
         <v>49</v>
@@ -13924,7 +13930,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="185" spans="1:13">
+    <row r="185" spans="1:13" hidden="1">
       <c r="A185" s="255"/>
       <c r="B185" s="145" t="s">
         <v>49</v>
@@ -13965,7 +13971,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="186" spans="1:13">
+    <row r="186" spans="1:13" hidden="1">
       <c r="A186" s="101" t="s">
         <v>50</v>
       </c>
@@ -14008,7 +14014,7 @@
         <v>CARMATEC IT SOLUTIONS PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="187" spans="1:13">
+    <row r="187" spans="1:13" hidden="1">
       <c r="A187" s="209" t="s">
         <v>52</v>
       </c>
@@ -14051,7 +14057,7 @@
         <v>Winnovation Education Services Pvt</v>
       </c>
     </row>
-    <row r="188" spans="1:13">
+    <row r="188" spans="1:13" hidden="1">
       <c r="A188" s="101" t="s">
         <v>50</v>
       </c>
@@ -14137,7 +14143,7 @@
         <v>BCT Consulting Private Limited</v>
       </c>
     </row>
-    <row r="190" spans="1:13">
+    <row r="190" spans="1:13" hidden="1">
       <c r="A190" s="257" t="s">
         <v>46</v>
       </c>
@@ -14180,7 +14186,7 @@
         <v>CANTICLE TECHNOLOGIES PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="191" spans="1:13">
+    <row r="191" spans="1:13" hidden="1">
       <c r="A191" s="149"/>
       <c r="B191" s="149" t="s">
         <v>72</v>
@@ -14224,7 +14230,7 @@
         <v>Cinesonic Audio Visual Pvt Ltd</v>
       </c>
     </row>
-    <row r="192" spans="1:13">
+    <row r="192" spans="1:13" hidden="1">
       <c r="A192" s="65"/>
       <c r="B192" s="65" t="s">
         <v>72</v>
@@ -14268,7 +14274,7 @@
         <v>Cinesonic Audio Visual Pvt Ltd</v>
       </c>
     </row>
-    <row r="193" spans="1:13">
+    <row r="193" spans="1:13" hidden="1">
       <c r="A193" s="65"/>
       <c r="B193" s="65" t="s">
         <v>72</v>
@@ -14312,7 +14318,7 @@
         <v>Cinesonic Audio Visual Pvt Ltd</v>
       </c>
     </row>
-    <row r="194" spans="1:13">
+    <row r="194" spans="1:13" hidden="1">
       <c r="A194" s="65"/>
       <c r="B194" s="65" t="s">
         <v>72</v>
@@ -14356,7 +14362,7 @@
         <v>Cinesonic Audio Visual Pvt Ltd</v>
       </c>
     </row>
-    <row r="195" spans="1:13">
+    <row r="195" spans="1:13" hidden="1">
       <c r="A195" s="65"/>
       <c r="B195" s="65" t="s">
         <v>72</v>
@@ -14400,7 +14406,7 @@
         <v>Cinesonic Audio Visual Pvt Ltd</v>
       </c>
     </row>
-    <row r="196" spans="1:13">
+    <row r="196" spans="1:13" hidden="1">
       <c r="A196" s="65"/>
       <c r="B196" s="65" t="s">
         <v>72</v>
@@ -14441,7 +14447,7 @@
         <v>Cinesonic Audio Visual Pvt Ltd</v>
       </c>
     </row>
-    <row r="197" spans="1:13">
+    <row r="197" spans="1:13" hidden="1">
       <c r="A197" s="65"/>
       <c r="B197" s="65" t="s">
         <v>72</v>
@@ -14482,7 +14488,7 @@
         <v>Cinesonic Audio Visual Pvt Ltd</v>
       </c>
     </row>
-    <row r="198" spans="1:13">
+    <row r="198" spans="1:13" hidden="1">
       <c r="A198" s="65"/>
       <c r="B198" s="65" t="s">
         <v>72</v>
@@ -14523,7 +14529,7 @@
         <v>Cinesonic Audio Visual Pvt Ltd</v>
       </c>
     </row>
-    <row r="199" spans="1:13">
+    <row r="199" spans="1:13" hidden="1">
       <c r="A199" s="65"/>
       <c r="B199" s="65" t="s">
         <v>72</v>
@@ -14564,7 +14570,7 @@
         <v>Cinesonic Audio Visual Pvt Ltd</v>
       </c>
     </row>
-    <row r="200" spans="1:13">
+    <row r="200" spans="1:13" hidden="1">
       <c r="A200" s="65"/>
       <c r="B200" s="65" t="s">
         <v>72</v>
@@ -14605,7 +14611,7 @@
         <v>Cinesonic Audio Visual Pvt Ltd</v>
       </c>
     </row>
-    <row r="201" spans="1:13">
+    <row r="201" spans="1:13" hidden="1">
       <c r="A201" s="65"/>
       <c r="B201" s="65" t="s">
         <v>72</v>
@@ -14646,7 +14652,7 @@
         <v>Cinesonic Audio Visual Pvt Ltd</v>
       </c>
     </row>
-    <row r="202" spans="1:13">
+    <row r="202" spans="1:13" hidden="1">
       <c r="A202" s="65"/>
       <c r="B202" s="65" t="s">
         <v>72</v>
@@ -14687,7 +14693,7 @@
         <v>Cinesonic Audio Visual Pvt Ltd</v>
       </c>
     </row>
-    <row r="203" spans="1:13">
+    <row r="203" spans="1:13" hidden="1">
       <c r="A203" s="65"/>
       <c r="B203" s="65" t="s">
         <v>72</v>
@@ -14728,7 +14734,7 @@
         <v>Cinesonic Audio Visual Pvt Ltd</v>
       </c>
     </row>
-    <row r="204" spans="1:13">
+    <row r="204" spans="1:13" hidden="1">
       <c r="A204" s="149"/>
       <c r="B204" s="148" t="s">
         <v>49</v>
@@ -14769,7 +14775,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="205" spans="1:13">
+    <row r="205" spans="1:13" hidden="1">
       <c r="A205" s="91" t="s">
         <v>427</v>
       </c>
@@ -14810,7 +14816,7 @@
         <v>Abhiyanta India Solution Private Limited</v>
       </c>
     </row>
-    <row r="206" spans="1:13">
+    <row r="206" spans="1:13" hidden="1">
       <c r="A206" s="91" t="s">
         <v>431</v>
       </c>
@@ -14851,7 +14857,7 @@
         <v>Abhiyanta India Solution Private Limited</v>
       </c>
     </row>
-    <row r="207" spans="1:13">
+    <row r="207" spans="1:13" hidden="1">
       <c r="A207" s="91" t="s">
         <v>433</v>
       </c>
@@ -14892,7 +14898,7 @@
         <v>Abhiyanta India Solution Private Limited</v>
       </c>
     </row>
-    <row r="208" spans="1:13">
+    <row r="208" spans="1:13" hidden="1">
       <c r="A208" s="257"/>
       <c r="B208" s="101" t="s">
         <v>196</v>
@@ -14931,7 +14937,7 @@
         <v>AUROPRO SOFT SYSTEMS PVT LTD</v>
       </c>
     </row>
-    <row r="209" spans="1:13">
+    <row r="209" spans="1:13" hidden="1">
       <c r="A209" s="91" t="s">
         <v>437</v>
       </c>
@@ -14974,7 +14980,7 @@
         <v>BCT Consulting Private Limited</v>
       </c>
     </row>
-    <row r="210" spans="1:13">
+    <row r="210" spans="1:13" hidden="1">
       <c r="A210" s="91" t="s">
         <v>437</v>
       </c>
@@ -15017,7 +15023,7 @@
         <v>BCT Consulting Private Limited</v>
       </c>
     </row>
-    <row r="211" spans="1:13">
+    <row r="211" spans="1:13" hidden="1">
       <c r="A211" s="164" t="s">
         <v>440</v>
       </c>
@@ -15058,7 +15064,7 @@
         <v>Abhiyanta India Solution Private Limited</v>
       </c>
     </row>
-    <row r="212" spans="1:13">
+    <row r="212" spans="1:13" hidden="1">
       <c r="A212" s="257" t="s">
         <v>46</v>
       </c>
@@ -15099,7 +15105,7 @@
         <v>CANTICLE TECHNOLOGIES PRIVATE LIMITED</v>
       </c>
     </row>
-    <row r="213" spans="1:13">
+    <row r="213" spans="1:13" hidden="1">
       <c r="A213" s="111" t="s">
         <v>71</v>
       </c>
@@ -15140,7 +15146,7 @@
         <v>ITSHRI SOLUTION LLP</v>
       </c>
     </row>
-    <row r="214" spans="1:13">
+    <row r="214" spans="1:13" hidden="1">
       <c r="A214" s="111" t="s">
         <v>71</v>
       </c>
@@ -15181,7 +15187,7 @@
         <v>ITSHRI SOLUTION LLP</v>
       </c>
     </row>
-    <row r="215" spans="1:13">
+    <row r="215" spans="1:13" hidden="1">
       <c r="A215" s="111" t="s">
         <v>71</v>
       </c>
@@ -15222,7 +15228,7 @@
         <v>ITSHRI SOLUTION LLP</v>
       </c>
     </row>
-    <row r="216" spans="1:13">
+    <row r="216" spans="1:13" hidden="1">
       <c r="A216" s="164" t="s">
         <v>446</v>
       </c>
@@ -15263,7 +15269,7 @@
         <v>Highsky IT Solutions Private Limited</v>
       </c>
     </row>
-    <row r="217" spans="1:13">
+    <row r="217" spans="1:13" hidden="1">
       <c r="A217" s="101" t="s">
         <v>50</v>
       </c>
@@ -15347,7 +15353,7 @@
         <v>BCT Consulting Private Limited</v>
       </c>
     </row>
-    <row r="219" spans="1:13">
+    <row r="219" spans="1:13" hidden="1">
       <c r="A219" s="257" t="s">
         <v>450</v>
       </c>
@@ -15389,7 +15395,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:M219" xr:uid="{2CD95930-0488-4552-AB38-23ACBD525592}"/>
+  <autoFilter ref="A2:M219" xr:uid="{2CD95930-0488-4552-AB38-23ACBD525592}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="4500095649"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -15397,11 +15409,12 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5351C4FA-754E-4B23-BAD5-F50DA5EFAFB9}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:S175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
+      <selection pane="bottomLeft" activeCell="I196" sqref="I196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
@@ -15441,25 +15454,25 @@
       <c r="K1" s="303"/>
       <c r="L1" s="92">
         <f>SUBTOTAL(9,L3:L1048576)</f>
-        <v>37936530.260000005</v>
+        <v>163548</v>
       </c>
       <c r="M1" s="93">
         <f>SUBTOTAL(9,M3:M1048576)</f>
-        <v>2764130.9132000003</v>
+        <v>3270.96</v>
       </c>
       <c r="N1" s="93">
         <f>SUBTOTAL(9,N3:N1048576)</f>
-        <v>42412454.793599993</v>
+        <v>189715.68</v>
       </c>
       <c r="O1" s="306"/>
       <c r="P1" s="92">
         <f>SUBTOTAL(9,P3:P1048576)</f>
-        <v>37766299.920000002</v>
+        <v>189715</v>
       </c>
       <c r="Q1" s="303"/>
       <c r="R1" s="92">
         <f>SUBTOTAL(9,R3:R1048576)</f>
-        <v>4646130.9655999988</v>
+        <v>0.68000000000029104</v>
       </c>
       <c r="S1" s="91"/>
     </row>
@@ -15699,7 +15712,7 @@
       </c>
       <c r="S5" s="91"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" hidden="1">
       <c r="A6" s="91" t="s">
         <v>41</v>
       </c>
@@ -15760,7 +15773,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" hidden="1">
       <c r="A7" s="91" t="s">
         <v>41</v>
       </c>
@@ -15821,7 +15834,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" hidden="1">
       <c r="A8" s="91" t="s">
         <v>44</v>
       </c>
@@ -15884,7 +15897,7 @@
       </c>
       <c r="S8" s="91"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" hidden="1">
       <c r="A9" s="91" t="s">
         <v>44</v>
       </c>
@@ -15947,7 +15960,7 @@
       </c>
       <c r="S9" s="91"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" hidden="1">
       <c r="A10" s="91" t="s">
         <v>44</v>
       </c>
@@ -16010,7 +16023,7 @@
       </c>
       <c r="S10" s="91"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" hidden="1">
       <c r="A11" s="91" t="s">
         <v>44</v>
       </c>
@@ -16073,7 +16086,7 @@
       </c>
       <c r="S11" s="91"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" hidden="1">
       <c r="A12" s="91" t="s">
         <v>44</v>
       </c>
@@ -16135,7 +16148,7 @@
       </c>
       <c r="S12" s="91"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" hidden="1">
       <c r="A13" s="91" t="s">
         <v>44</v>
       </c>
@@ -16199,7 +16212,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" hidden="1">
       <c r="A14" s="91" t="s">
         <v>44</v>
       </c>
@@ -16263,7 +16276,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" hidden="1">
       <c r="A15" s="91" t="s">
         <v>46</v>
       </c>
@@ -16323,7 +16336,7 @@
       </c>
       <c r="S15" s="91"/>
     </row>
-    <row r="16" spans="1:19" ht="14.4">
+    <row r="16" spans="1:19" ht="14.4" hidden="1">
       <c r="A16" s="91" t="s">
         <v>482</v>
       </c>
@@ -16378,7 +16391,7 @@
       </c>
       <c r="S16" s="91"/>
     </row>
-    <row r="17" spans="1:19" ht="14.4">
+    <row r="17" spans="1:19" ht="14.4" hidden="1">
       <c r="A17" s="91" t="s">
         <v>482</v>
       </c>
@@ -16433,7 +16446,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="14.4">
+    <row r="18" spans="1:19" ht="14.4" hidden="1">
       <c r="A18" s="91" t="s">
         <v>482</v>
       </c>
@@ -16489,7 +16502,7 @@
       </c>
       <c r="S18" s="91"/>
     </row>
-    <row r="19" spans="1:19" ht="14.4">
+    <row r="19" spans="1:19" ht="14.4" hidden="1">
       <c r="A19" s="91" t="s">
         <v>482</v>
       </c>
@@ -16545,7 +16558,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" hidden="1">
       <c r="A20" s="91" t="s">
         <v>48</v>
       </c>
@@ -16605,7 +16618,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" hidden="1">
       <c r="A21" s="97" t="s">
         <v>50</v>
       </c>
@@ -16664,7 +16677,7 @@
       </c>
       <c r="S21" s="91"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" hidden="1">
       <c r="A22" s="97" t="s">
         <v>50</v>
       </c>
@@ -16723,7 +16736,7 @@
       </c>
       <c r="S22" s="91"/>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" hidden="1">
       <c r="A23" s="97" t="s">
         <v>50</v>
       </c>
@@ -16782,7 +16795,7 @@
       </c>
       <c r="S23" s="91"/>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" hidden="1">
       <c r="A24" s="97" t="s">
         <v>50</v>
       </c>
@@ -16841,7 +16854,7 @@
       </c>
       <c r="S24" s="91"/>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" hidden="1">
       <c r="A25" s="97" t="s">
         <v>50</v>
       </c>
@@ -16900,7 +16913,7 @@
       </c>
       <c r="S25" s="91"/>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" hidden="1">
       <c r="A26" s="97" t="s">
         <v>50</v>
       </c>
@@ -16961,7 +16974,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" hidden="1">
       <c r="A27" s="97" t="s">
         <v>50</v>
       </c>
@@ -17022,7 +17035,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" hidden="1">
       <c r="A28" s="97" t="s">
         <v>52</v>
       </c>
@@ -17079,7 +17092,7 @@
       </c>
       <c r="S28" s="91"/>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" hidden="1">
       <c r="A29" s="97" t="s">
         <v>52</v>
       </c>
@@ -17136,7 +17149,7 @@
       </c>
       <c r="S29" s="91"/>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" hidden="1">
       <c r="A30" s="97" t="s">
         <v>52</v>
       </c>
@@ -17193,7 +17206,7 @@
       </c>
       <c r="S30" s="97"/>
     </row>
-    <row r="31" spans="1:19" ht="14.4">
+    <row r="31" spans="1:19" ht="14.4" hidden="1">
       <c r="A31" s="97" t="s">
         <v>52</v>
       </c>
@@ -17248,7 +17261,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" hidden="1">
       <c r="A32" s="91" t="s">
         <v>53</v>
       </c>
@@ -17305,7 +17318,7 @@
       </c>
       <c r="S32" s="91"/>
     </row>
-    <row r="33" spans="1:19">
+    <row r="33" spans="1:19" hidden="1">
       <c r="A33" s="91" t="s">
         <v>53</v>
       </c>
@@ -17362,7 +17375,7 @@
       </c>
       <c r="S33" s="91"/>
     </row>
-    <row r="34" spans="1:19" ht="14.4">
+    <row r="34" spans="1:19" ht="14.4" hidden="1">
       <c r="A34" s="91" t="s">
         <v>53</v>
       </c>
@@ -17419,7 +17432,7 @@
       </c>
       <c r="S34" s="91"/>
     </row>
-    <row r="35" spans="1:19">
+    <row r="35" spans="1:19" hidden="1">
       <c r="A35" s="91" t="s">
         <v>53</v>
       </c>
@@ -17476,7 +17489,7 @@
       </c>
       <c r="S35" s="91"/>
     </row>
-    <row r="36" spans="1:19">
+    <row r="36" spans="1:19" hidden="1">
       <c r="A36" s="91" t="s">
         <v>54</v>
       </c>
@@ -17534,7 +17547,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="1:19" hidden="1">
       <c r="A37" s="91" t="s">
         <v>54</v>
       </c>
@@ -17592,7 +17605,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="38" spans="1:19">
+    <row r="38" spans="1:19" hidden="1">
       <c r="A38" s="91" t="s">
         <v>54</v>
       </c>
@@ -17650,7 +17663,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="39" spans="1:19">
+    <row r="39" spans="1:19" hidden="1">
       <c r="A39" s="91" t="s">
         <v>54</v>
       </c>
@@ -17708,7 +17721,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="40" spans="1:19">
+    <row r="40" spans="1:19" hidden="1">
       <c r="A40" s="91" t="s">
         <v>54</v>
       </c>
@@ -17766,7 +17779,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="41" spans="1:19">
+    <row r="41" spans="1:19" hidden="1">
       <c r="A41" s="91" t="s">
         <v>54</v>
       </c>
@@ -17824,7 +17837,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="42" spans="1:19">
+    <row r="42" spans="1:19" hidden="1">
       <c r="A42" s="91" t="s">
         <v>54</v>
       </c>
@@ -17882,7 +17895,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="43" spans="1:19">
+    <row r="43" spans="1:19" hidden="1">
       <c r="A43" s="91" t="s">
         <v>54</v>
       </c>
@@ -17940,7 +17953,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="44" spans="1:19">
+    <row r="44" spans="1:19" hidden="1">
       <c r="A44" s="91"/>
       <c r="B44" s="97"/>
       <c r="C44" s="97"/>
@@ -17977,7 +17990,7 @@
       </c>
       <c r="S44" s="97"/>
     </row>
-    <row r="45" spans="1:19">
+    <row r="45" spans="1:19" hidden="1">
       <c r="A45" s="91"/>
       <c r="B45" s="97" t="s">
         <v>56</v>
@@ -18025,7 +18038,7 @@
       </c>
       <c r="S45" s="91"/>
     </row>
-    <row r="46" spans="1:19">
+    <row r="46" spans="1:19" hidden="1">
       <c r="A46" s="91"/>
       <c r="B46" s="97" t="s">
         <v>57</v>
@@ -18073,7 +18086,7 @@
       </c>
       <c r="S46" s="91"/>
     </row>
-    <row r="47" spans="1:19">
+    <row r="47" spans="1:19" hidden="1">
       <c r="A47" s="91"/>
       <c r="B47" s="97" t="s">
         <v>57</v>
@@ -18121,7 +18134,7 @@
       </c>
       <c r="S47" s="91"/>
     </row>
-    <row r="48" spans="1:19">
+    <row r="48" spans="1:19" hidden="1">
       <c r="A48" s="91"/>
       <c r="B48" s="97" t="s">
         <v>56</v>
@@ -18170,7 +18183,7 @@
       </c>
       <c r="S48" s="91"/>
     </row>
-    <row r="49" spans="1:19">
+    <row r="49" spans="1:19" hidden="1">
       <c r="A49" s="91"/>
       <c r="B49" s="97" t="s">
         <v>57</v>
@@ -18218,7 +18231,7 @@
       </c>
       <c r="S49" s="91"/>
     </row>
-    <row r="50" spans="1:19">
+    <row r="50" spans="1:19" hidden="1">
       <c r="A50" s="91"/>
       <c r="B50" s="97" t="s">
         <v>57</v>
@@ -18266,7 +18279,7 @@
       </c>
       <c r="S50" s="91"/>
     </row>
-    <row r="51" spans="1:19">
+    <row r="51" spans="1:19" hidden="1">
       <c r="A51" s="91"/>
       <c r="B51" s="97" t="s">
         <v>57</v>
@@ -18314,7 +18327,7 @@
       </c>
       <c r="S51" s="91"/>
     </row>
-    <row r="52" spans="1:19">
+    <row r="52" spans="1:19" hidden="1">
       <c r="A52" s="91"/>
       <c r="B52" s="97" t="s">
         <v>57</v>
@@ -18362,7 +18375,7 @@
       </c>
       <c r="S52" s="91"/>
     </row>
-    <row r="53" spans="1:19">
+    <row r="53" spans="1:19" hidden="1">
       <c r="A53" s="91"/>
       <c r="B53" s="97" t="s">
         <v>57</v>
@@ -18410,7 +18423,7 @@
       </c>
       <c r="S53" s="91"/>
     </row>
-    <row r="54" spans="1:19">
+    <row r="54" spans="1:19" hidden="1">
       <c r="A54" s="91"/>
       <c r="B54" s="97" t="s">
         <v>57</v>
@@ -18458,7 +18471,7 @@
       </c>
       <c r="S54" s="91"/>
     </row>
-    <row r="55" spans="1:19">
+    <row r="55" spans="1:19" hidden="1">
       <c r="A55" s="91"/>
       <c r="B55" s="97" t="s">
         <v>56</v>
@@ -18506,7 +18519,7 @@
       </c>
       <c r="S55" s="91"/>
     </row>
-    <row r="56" spans="1:19">
+    <row r="56" spans="1:19" hidden="1">
       <c r="A56" s="91"/>
       <c r="B56" s="97" t="s">
         <v>56</v>
@@ -18555,7 +18568,7 @@
       </c>
       <c r="S56" s="91"/>
     </row>
-    <row r="57" spans="1:19">
+    <row r="57" spans="1:19" hidden="1">
       <c r="A57" s="91"/>
       <c r="B57" s="97" t="s">
         <v>57</v>
@@ -18603,7 +18616,7 @@
       </c>
       <c r="S57" s="91"/>
     </row>
-    <row r="58" spans="1:19">
+    <row r="58" spans="1:19" hidden="1">
       <c r="A58" s="91"/>
       <c r="B58" s="97" t="s">
         <v>58</v>
@@ -18651,7 +18664,7 @@
       </c>
       <c r="S58" s="91"/>
     </row>
-    <row r="59" spans="1:19">
+    <row r="59" spans="1:19" hidden="1">
       <c r="A59" s="91"/>
       <c r="B59" s="97" t="s">
         <v>58</v>
@@ -18699,7 +18712,7 @@
       </c>
       <c r="S59" s="91"/>
     </row>
-    <row r="60" spans="1:19">
+    <row r="60" spans="1:19" hidden="1">
       <c r="A60" s="91"/>
       <c r="B60" s="97" t="s">
         <v>58</v>
@@ -18747,7 +18760,7 @@
       </c>
       <c r="S60" s="91"/>
     </row>
-    <row r="61" spans="1:19">
+    <row r="61" spans="1:19" hidden="1">
       <c r="A61" s="91"/>
       <c r="B61" s="97" t="s">
         <v>57</v>
@@ -18795,7 +18808,7 @@
       </c>
       <c r="S61" s="91"/>
     </row>
-    <row r="62" spans="1:19">
+    <row r="62" spans="1:19" hidden="1">
       <c r="A62" s="91"/>
       <c r="B62" s="97" t="s">
         <v>57</v>
@@ -18843,7 +18856,7 @@
       </c>
       <c r="S62" s="91"/>
     </row>
-    <row r="63" spans="1:19">
+    <row r="63" spans="1:19" hidden="1">
       <c r="A63" s="91"/>
       <c r="B63" s="97" t="s">
         <v>57</v>
@@ -18892,7 +18905,7 @@
       </c>
       <c r="S63" s="91"/>
     </row>
-    <row r="64" spans="1:19">
+    <row r="64" spans="1:19" hidden="1">
       <c r="A64" s="91"/>
       <c r="B64" s="97" t="s">
         <v>56</v>
@@ -18940,7 +18953,7 @@
       </c>
       <c r="S64" s="91"/>
     </row>
-    <row r="65" spans="1:19">
+    <row r="65" spans="1:19" hidden="1">
       <c r="A65" s="91"/>
       <c r="B65" s="97" t="s">
         <v>57</v>
@@ -18988,7 +19001,7 @@
       </c>
       <c r="S65" s="91"/>
     </row>
-    <row r="66" spans="1:19">
+    <row r="66" spans="1:19" hidden="1">
       <c r="A66" s="91"/>
       <c r="B66" s="97" t="s">
         <v>57</v>
@@ -19037,7 +19050,7 @@
       </c>
       <c r="S66" s="91"/>
     </row>
-    <row r="67" spans="1:19">
+    <row r="67" spans="1:19" hidden="1">
       <c r="A67" s="91"/>
       <c r="B67" s="97" t="s">
         <v>57</v>
@@ -19087,7 +19100,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="68" spans="1:19">
+    <row r="68" spans="1:19" hidden="1">
       <c r="A68" s="91"/>
       <c r="B68" s="97" t="s">
         <v>56</v>
@@ -19135,7 +19148,7 @@
       </c>
       <c r="S68" s="91"/>
     </row>
-    <row r="69" spans="1:19">
+    <row r="69" spans="1:19" hidden="1">
       <c r="A69" s="91"/>
       <c r="B69" s="97" t="s">
         <v>236</v>
@@ -19183,7 +19196,7 @@
       </c>
       <c r="S69" s="91"/>
     </row>
-    <row r="70" spans="1:19">
+    <row r="70" spans="1:19" hidden="1">
       <c r="A70" s="91"/>
       <c r="B70" s="97" t="s">
         <v>74</v>
@@ -19232,7 +19245,7 @@
       </c>
       <c r="S70" s="91"/>
     </row>
-    <row r="71" spans="1:19" ht="14.4">
+    <row r="71" spans="1:19" ht="14.4" hidden="1">
       <c r="A71" s="91"/>
       <c r="B71" s="97" t="s">
         <v>74</v>
@@ -19282,7 +19295,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="72" spans="1:19">
+    <row r="72" spans="1:19" hidden="1">
       <c r="A72" s="91"/>
       <c r="B72" s="97" t="s">
         <v>74</v>
@@ -19330,7 +19343,7 @@
       </c>
       <c r="S72" s="91"/>
     </row>
-    <row r="73" spans="1:19">
+    <row r="73" spans="1:19" hidden="1">
       <c r="A73" s="91"/>
       <c r="B73" s="97" t="s">
         <v>74</v>
@@ -19378,7 +19391,7 @@
       </c>
       <c r="S73" s="91"/>
     </row>
-    <row r="74" spans="1:19">
+    <row r="74" spans="1:19" hidden="1">
       <c r="A74" s="105"/>
       <c r="B74" s="105" t="s">
         <v>74</v>
@@ -19428,7 +19441,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="75" spans="1:19">
+    <row r="75" spans="1:19" hidden="1">
       <c r="A75" s="105"/>
       <c r="B75" s="105" t="s">
         <v>74</v>
@@ -19478,7 +19491,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="76" spans="1:19">
+    <row r="76" spans="1:19" hidden="1">
       <c r="A76" s="91"/>
       <c r="B76" s="97" t="s">
         <v>74</v>
@@ -19528,7 +19541,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="14.4">
+    <row r="77" spans="1:19" ht="14.4" hidden="1">
       <c r="A77" s="91"/>
       <c r="B77" s="97" t="s">
         <v>74</v>
@@ -19576,7 +19589,7 @@
       </c>
       <c r="S77" s="91"/>
     </row>
-    <row r="78" spans="1:19" ht="14.4">
+    <row r="78" spans="1:19" ht="14.4" hidden="1">
       <c r="A78" s="91"/>
       <c r="B78" s="97" t="s">
         <v>74</v>
@@ -19624,7 +19637,7 @@
       </c>
       <c r="S78" s="91"/>
     </row>
-    <row r="79" spans="1:19">
+    <row r="79" spans="1:19" hidden="1">
       <c r="A79" s="91"/>
       <c r="B79" s="97" t="s">
         <v>247</v>
@@ -19673,7 +19686,7 @@
       </c>
       <c r="S79" s="91"/>
     </row>
-    <row r="80" spans="1:19" ht="14.4">
+    <row r="80" spans="1:19" ht="14.4" hidden="1">
       <c r="A80" s="91"/>
       <c r="B80" s="97" t="s">
         <v>74</v>
@@ -19721,7 +19734,7 @@
       </c>
       <c r="S80" s="91"/>
     </row>
-    <row r="81" spans="1:19" ht="14.4">
+    <row r="81" spans="1:19" ht="14.4" hidden="1">
       <c r="A81" s="91"/>
       <c r="B81" s="97" t="s">
         <v>74</v>
@@ -19769,7 +19782,7 @@
       </c>
       <c r="S81" s="91"/>
     </row>
-    <row r="82" spans="1:19" ht="14.4">
+    <row r="82" spans="1:19" ht="14.4" hidden="1">
       <c r="A82" s="91"/>
       <c r="B82" s="97" t="s">
         <v>247</v>
@@ -19817,7 +19830,7 @@
       </c>
       <c r="S82" s="91"/>
     </row>
-    <row r="83" spans="1:19" ht="14.4">
+    <row r="83" spans="1:19" ht="14.4" hidden="1">
       <c r="A83" s="91"/>
       <c r="B83" s="97" t="s">
         <v>247</v>
@@ -19866,7 +19879,7 @@
       </c>
       <c r="S83" s="91"/>
     </row>
-    <row r="84" spans="1:19" ht="14.4">
+    <row r="84" spans="1:19" ht="14.4" hidden="1">
       <c r="A84" s="91"/>
       <c r="B84" s="97" t="s">
         <v>74</v>
@@ -19914,7 +19927,7 @@
       </c>
       <c r="S84" s="91"/>
     </row>
-    <row r="85" spans="1:19" ht="14.4">
+    <row r="85" spans="1:19" ht="14.4" hidden="1">
       <c r="A85" s="91"/>
       <c r="B85" s="97" t="s">
         <v>74</v>
@@ -19962,7 +19975,7 @@
       </c>
       <c r="S85" s="91"/>
     </row>
-    <row r="86" spans="1:19" ht="14.4">
+    <row r="86" spans="1:19" ht="14.4" hidden="1">
       <c r="A86" s="91"/>
       <c r="B86" s="97" t="s">
         <v>247</v>
@@ -20013,7 +20026,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="87" spans="1:19">
+    <row r="87" spans="1:19" hidden="1">
       <c r="A87" s="91"/>
       <c r="B87" s="97" t="s">
         <v>74</v>
@@ -20059,7 +20072,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="88" spans="1:19">
+    <row r="88" spans="1:19" hidden="1">
       <c r="A88" s="91"/>
       <c r="B88" s="97" t="s">
         <v>74</v>
@@ -20105,7 +20118,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="89" spans="1:19">
+    <row r="89" spans="1:19" hidden="1">
       <c r="A89" s="91"/>
       <c r="B89" s="97" t="s">
         <v>74</v>
@@ -20151,7 +20164,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="90" spans="1:19">
+    <row r="90" spans="1:19" hidden="1">
       <c r="A90" s="91"/>
       <c r="B90" s="97" t="s">
         <v>74</v>
@@ -20197,7 +20210,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="91" spans="1:19">
+    <row r="91" spans="1:19" hidden="1">
       <c r="A91" s="91"/>
       <c r="B91" s="97" t="s">
         <v>74</v>
@@ -20243,7 +20256,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="92" spans="1:19">
+    <row r="92" spans="1:19" hidden="1">
       <c r="A92" s="91"/>
       <c r="B92" s="97" t="s">
         <v>74</v>
@@ -20289,7 +20302,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="93" spans="1:19">
+    <row r="93" spans="1:19" hidden="1">
       <c r="A93" s="91"/>
       <c r="B93" s="97" t="s">
         <v>74</v>
@@ -20335,7 +20348,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="94" spans="1:19">
+    <row r="94" spans="1:19" hidden="1">
       <c r="A94" s="91"/>
       <c r="B94" s="97" t="s">
         <v>74</v>
@@ -20381,7 +20394,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="95" spans="1:19">
+    <row r="95" spans="1:19" hidden="1">
       <c r="A95" s="91"/>
       <c r="B95" s="97" t="s">
         <v>74</v>
@@ -20427,7 +20440,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="96" spans="1:19">
+    <row r="96" spans="1:19" hidden="1">
       <c r="A96" s="91"/>
       <c r="B96" s="97" t="s">
         <v>74</v>
@@ -20473,7 +20486,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="97" spans="1:19">
+    <row r="97" spans="1:19" hidden="1">
       <c r="A97" s="91"/>
       <c r="B97" s="97" t="s">
         <v>74</v>
@@ -20519,7 +20532,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="98" spans="1:19">
+    <row r="98" spans="1:19" hidden="1">
       <c r="A98" s="91"/>
       <c r="B98" s="97" t="s">
         <v>74</v>
@@ -20565,7 +20578,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="99" spans="1:19">
+    <row r="99" spans="1:19" hidden="1">
       <c r="A99" s="91"/>
       <c r="B99" s="97" t="s">
         <v>74</v>
@@ -20611,7 +20624,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="100" spans="1:19">
+    <row r="100" spans="1:19" hidden="1">
       <c r="A100" s="91"/>
       <c r="B100" s="97" t="s">
         <v>74</v>
@@ -20657,7 +20670,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="101" spans="1:19">
+    <row r="101" spans="1:19" hidden="1">
       <c r="A101" s="91"/>
       <c r="B101" s="97" t="s">
         <v>74</v>
@@ -20703,7 +20716,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="102" spans="1:19">
+    <row r="102" spans="1:19" hidden="1">
       <c r="A102" s="91"/>
       <c r="B102" s="97" t="s">
         <v>74</v>
@@ -20749,7 +20762,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="103" spans="1:19">
+    <row r="103" spans="1:19" hidden="1">
       <c r="A103" s="91"/>
       <c r="B103" s="97" t="s">
         <v>74</v>
@@ -20795,7 +20808,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="104" spans="1:19">
+    <row r="104" spans="1:19" hidden="1">
       <c r="A104" s="91"/>
       <c r="B104" s="97" t="s">
         <v>74</v>
@@ -20841,7 +20854,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="105" spans="1:19">
+    <row r="105" spans="1:19" hidden="1">
       <c r="A105" s="91"/>
       <c r="B105" s="97" t="s">
         <v>74</v>
@@ -20887,7 +20900,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="106" spans="1:19">
+    <row r="106" spans="1:19" hidden="1">
       <c r="A106" s="91"/>
       <c r="B106" s="97" t="s">
         <v>74</v>
@@ -20933,7 +20946,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="107" spans="1:19">
+    <row r="107" spans="1:19" hidden="1">
       <c r="A107" s="91"/>
       <c r="B107" s="97" t="s">
         <v>74</v>
@@ -20979,7 +20992,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="108" spans="1:19">
+    <row r="108" spans="1:19" hidden="1">
       <c r="A108" s="91"/>
       <c r="B108" s="97" t="s">
         <v>74</v>
@@ -21025,7 +21038,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="109" spans="1:19">
+    <row r="109" spans="1:19" hidden="1">
       <c r="A109" s="91"/>
       <c r="B109" s="97" t="s">
         <v>74</v>
@@ -21071,7 +21084,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="110" spans="1:19">
+    <row r="110" spans="1:19" hidden="1">
       <c r="A110" s="91"/>
       <c r="B110" s="97" t="s">
         <v>74</v>
@@ -21117,7 +21130,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="111" spans="1:19">
+    <row r="111" spans="1:19" hidden="1">
       <c r="A111" s="91"/>
       <c r="B111" s="97" t="s">
         <v>74</v>
@@ -21163,7 +21176,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="112" spans="1:19">
+    <row r="112" spans="1:19" hidden="1">
       <c r="A112" s="91"/>
       <c r="B112" s="97" t="s">
         <v>74</v>
@@ -21209,7 +21222,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="113" spans="1:19">
+    <row r="113" spans="1:19" hidden="1">
       <c r="A113" s="91"/>
       <c r="B113" s="97" t="s">
         <v>74</v>
@@ -21255,7 +21268,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="114" spans="1:19">
+    <row r="114" spans="1:19" hidden="1">
       <c r="A114" s="91"/>
       <c r="B114" s="97" t="s">
         <v>74</v>
@@ -21301,7 +21314,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="115" spans="1:19">
+    <row r="115" spans="1:19" hidden="1">
       <c r="A115" s="91"/>
       <c r="B115" s="97" t="s">
         <v>74</v>
@@ -21347,7 +21360,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="116" spans="1:19">
+    <row r="116" spans="1:19" hidden="1">
       <c r="A116" s="91"/>
       <c r="B116" s="97" t="s">
         <v>74</v>
@@ -21393,7 +21406,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="117" spans="1:19">
+    <row r="117" spans="1:19" hidden="1">
       <c r="A117" s="91"/>
       <c r="B117" s="97" t="s">
         <v>74</v>
@@ -21439,7 +21452,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="118" spans="1:19">
+    <row r="118" spans="1:19" hidden="1">
       <c r="A118" s="91"/>
       <c r="B118" s="97" t="s">
         <v>74</v>
@@ -21485,7 +21498,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="119" spans="1:19">
+    <row r="119" spans="1:19" hidden="1">
       <c r="A119" s="91"/>
       <c r="B119" s="97" t="s">
         <v>74</v>
@@ -21531,7 +21544,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="120" spans="1:19">
+    <row r="120" spans="1:19" hidden="1">
       <c r="A120" s="91"/>
       <c r="B120" s="97" t="s">
         <v>74</v>
@@ -21577,7 +21590,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="121" spans="1:19">
+    <row r="121" spans="1:19" hidden="1">
       <c r="A121" s="91"/>
       <c r="B121" s="97" t="s">
         <v>74</v>
@@ -21623,7 +21636,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="122" spans="1:19">
+    <row r="122" spans="1:19" hidden="1">
       <c r="A122" s="91"/>
       <c r="B122" s="97" t="s">
         <v>74</v>
@@ -21669,7 +21682,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="123" spans="1:19">
+    <row r="123" spans="1:19" hidden="1">
       <c r="A123" s="91"/>
       <c r="B123" s="97" t="s">
         <v>74</v>
@@ -21715,7 +21728,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="124" spans="1:19">
+    <row r="124" spans="1:19" hidden="1">
       <c r="A124" s="91"/>
       <c r="B124" s="97" t="s">
         <v>74</v>
@@ -21761,7 +21774,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="125" spans="1:19">
+    <row r="125" spans="1:19" hidden="1">
       <c r="A125" s="91"/>
       <c r="B125" s="97" t="s">
         <v>74</v>
@@ -21807,7 +21820,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="126" spans="1:19">
+    <row r="126" spans="1:19" hidden="1">
       <c r="A126" s="91"/>
       <c r="B126" s="97" t="s">
         <v>74</v>
@@ -21853,7 +21866,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="127" spans="1:19">
+    <row r="127" spans="1:19" hidden="1">
       <c r="A127" s="91"/>
       <c r="B127" s="97" t="s">
         <v>74</v>
@@ -21899,7 +21912,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="128" spans="1:19">
+    <row r="128" spans="1:19" hidden="1">
       <c r="A128" s="91"/>
       <c r="B128" s="97" t="s">
         <v>74</v>
@@ -21945,7 +21958,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="129" spans="1:19">
+    <row r="129" spans="1:19" hidden="1">
       <c r="A129" s="91"/>
       <c r="B129" s="97" t="s">
         <v>74</v>
@@ -21991,7 +22004,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="130" spans="1:19">
+    <row r="130" spans="1:19" hidden="1">
       <c r="A130" s="91"/>
       <c r="B130" s="97" t="s">
         <v>74</v>
@@ -22037,7 +22050,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="131" spans="1:19">
+    <row r="131" spans="1:19" hidden="1">
       <c r="A131" s="91"/>
       <c r="B131" s="97" t="s">
         <v>74</v>
@@ -22083,7 +22096,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="132" spans="1:19">
+    <row r="132" spans="1:19" hidden="1">
       <c r="A132" s="91"/>
       <c r="B132" s="97" t="s">
         <v>74</v>
@@ -22129,7 +22142,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="133" spans="1:19">
+    <row r="133" spans="1:19" hidden="1">
       <c r="A133" s="91"/>
       <c r="B133" s="97" t="s">
         <v>74</v>
@@ -22175,7 +22188,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="134" spans="1:19">
+    <row r="134" spans="1:19" hidden="1">
       <c r="A134" s="91"/>
       <c r="B134" s="97" t="s">
         <v>74</v>
@@ -22221,7 +22234,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="135" spans="1:19">
+    <row r="135" spans="1:19" hidden="1">
       <c r="A135" s="91"/>
       <c r="B135" s="97" t="s">
         <v>74</v>
@@ -22267,7 +22280,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="136" spans="1:19">
+    <row r="136" spans="1:19" hidden="1">
       <c r="A136" s="91"/>
       <c r="B136" s="97" t="s">
         <v>74</v>
@@ -22313,7 +22326,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="137" spans="1:19">
+    <row r="137" spans="1:19" hidden="1">
       <c r="A137" s="91"/>
       <c r="B137" s="97" t="s">
         <v>74</v>
@@ -22359,7 +22372,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="138" spans="1:19">
+    <row r="138" spans="1:19" hidden="1">
       <c r="A138" s="91"/>
       <c r="B138" s="97" t="s">
         <v>74</v>
@@ -22405,7 +22418,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="139" spans="1:19">
+    <row r="139" spans="1:19" hidden="1">
       <c r="A139" s="91"/>
       <c r="B139" s="97" t="s">
         <v>74</v>
@@ -22451,7 +22464,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="140" spans="1:19">
+    <row r="140" spans="1:19" hidden="1">
       <c r="A140" s="91"/>
       <c r="B140" s="97" t="s">
         <v>74</v>
@@ -22497,7 +22510,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="141" spans="1:19">
+    <row r="141" spans="1:19" hidden="1">
       <c r="A141" s="91"/>
       <c r="B141" s="97" t="s">
         <v>74</v>
@@ -22543,7 +22556,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="142" spans="1:19">
+    <row r="142" spans="1:19" hidden="1">
       <c r="A142" s="91"/>
       <c r="B142" s="97" t="s">
         <v>74</v>
@@ -22589,7 +22602,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="143" spans="1:19">
+    <row r="143" spans="1:19" hidden="1">
       <c r="A143" s="91"/>
       <c r="B143" s="97" t="s">
         <v>74</v>
@@ -22635,7 +22648,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="144" spans="1:19">
+    <row r="144" spans="1:19" hidden="1">
       <c r="A144" s="91"/>
       <c r="B144" s="97" t="s">
         <v>74</v>
@@ -22681,7 +22694,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="145" spans="1:19">
+    <row r="145" spans="1:19" hidden="1">
       <c r="A145" s="91"/>
       <c r="B145" s="97" t="s">
         <v>74</v>
@@ -22727,7 +22740,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="146" spans="1:19">
+    <row r="146" spans="1:19" hidden="1">
       <c r="A146" s="91"/>
       <c r="B146" s="97" t="s">
         <v>74</v>
@@ -22773,7 +22786,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="147" spans="1:19">
+    <row r="147" spans="1:19" hidden="1">
       <c r="A147" s="91"/>
       <c r="B147" s="97" t="s">
         <v>74</v>
@@ -22819,7 +22832,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="148" spans="1:19">
+    <row r="148" spans="1:19" hidden="1">
       <c r="A148" s="157" t="s">
         <v>73</v>
       </c>
@@ -22875,7 +22888,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="149" spans="1:19">
+    <row r="149" spans="1:19" hidden="1">
       <c r="A149" s="91"/>
       <c r="B149" s="97" t="s">
         <v>74</v>
@@ -22919,7 +22932,7 @@
       </c>
       <c r="S149" s="91"/>
     </row>
-    <row r="150" spans="1:19">
+    <row r="150" spans="1:19" hidden="1">
       <c r="A150" s="91"/>
       <c r="B150" s="97" t="s">
         <v>74</v>
@@ -22963,7 +22976,7 @@
       </c>
       <c r="S150" s="91"/>
     </row>
-    <row r="151" spans="1:19">
+    <row r="151" spans="1:19" hidden="1">
       <c r="A151" s="91"/>
       <c r="B151" s="97" t="s">
         <v>61</v>
@@ -23020,7 +23033,7 @@
       </c>
       <c r="S151" s="91"/>
     </row>
-    <row r="152" spans="1:19">
+    <row r="152" spans="1:19" hidden="1">
       <c r="A152" s="91" t="s">
         <v>46</v>
       </c>
@@ -23081,7 +23094,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="153" spans="1:19">
+    <row r="153" spans="1:19" hidden="1">
       <c r="A153" s="91" t="s">
         <v>54</v>
       </c>
@@ -23139,7 +23152,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="154" spans="1:19">
+    <row r="154" spans="1:19" hidden="1">
       <c r="A154" s="97" t="s">
         <v>50</v>
       </c>
@@ -23200,7 +23213,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="155" spans="1:19">
+    <row r="155" spans="1:19" hidden="1">
       <c r="A155" s="91" t="s">
         <v>44</v>
       </c>
@@ -23264,7 +23277,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="156" spans="1:19">
+    <row r="156" spans="1:19" hidden="1">
       <c r="A156" s="91" t="s">
         <v>446</v>
       </c>
@@ -23323,7 +23336,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="157" spans="1:19">
+    <row r="157" spans="1:19" hidden="1">
       <c r="A157" s="91" t="s">
         <v>606</v>
       </c>
@@ -23378,7 +23391,7 @@
       </c>
       <c r="S157" s="91"/>
     </row>
-    <row r="158" spans="1:19">
+    <row r="158" spans="1:19" hidden="1">
       <c r="A158" s="91" t="s">
         <v>450</v>
       </c>
@@ -23433,7 +23446,7 @@
       </c>
       <c r="S158" s="91"/>
     </row>
-    <row r="159" spans="1:19">
+    <row r="159" spans="1:19" hidden="1">
       <c r="A159" s="91" t="s">
         <v>437</v>
       </c>
@@ -23488,7 +23501,7 @@
       </c>
       <c r="S159" s="91"/>
     </row>
-    <row r="160" spans="1:19">
+    <row r="160" spans="1:19" hidden="1">
       <c r="A160" s="91" t="s">
         <v>614</v>
       </c>
@@ -23543,7 +23556,7 @@
       </c>
       <c r="S160" s="91"/>
     </row>
-    <row r="161" spans="1:19">
+    <row r="161" spans="1:19" hidden="1">
       <c r="A161" s="91" t="s">
         <v>70</v>
       </c>
@@ -23596,7 +23609,7 @@
       </c>
       <c r="S161" s="91"/>
     </row>
-    <row r="162" spans="1:19" ht="14.4">
+    <row r="162" spans="1:19" ht="14.4" hidden="1">
       <c r="A162" s="111" t="s">
         <v>71</v>
       </c>
@@ -23651,7 +23664,7 @@
       </c>
       <c r="S162" s="91"/>
     </row>
-    <row r="163" spans="1:19">
+    <row r="163" spans="1:19" hidden="1">
       <c r="A163" s="91" t="s">
         <v>624</v>
       </c>
@@ -23706,7 +23719,7 @@
       </c>
       <c r="S163" s="91"/>
     </row>
-    <row r="164" spans="1:19">
+    <row r="164" spans="1:19" hidden="1">
       <c r="A164" s="91" t="s">
         <v>625</v>
       </c>
@@ -23761,7 +23774,7 @@
       </c>
       <c r="S164" s="91"/>
     </row>
-    <row r="165" spans="1:19" ht="14.4">
+    <row r="165" spans="1:19" ht="14.4" hidden="1">
       <c r="A165" s="111" t="s">
         <v>71</v>
       </c>
@@ -23816,7 +23829,7 @@
       </c>
       <c r="S165" s="91"/>
     </row>
-    <row r="166" spans="1:19" ht="14.4">
+    <row r="166" spans="1:19" ht="14.4" hidden="1">
       <c r="A166" s="193" t="s">
         <v>71</v>
       </c>
@@ -23871,7 +23884,7 @@
       </c>
       <c r="S166" s="91"/>
     </row>
-    <row r="167" spans="1:19">
+    <row r="167" spans="1:19" hidden="1">
       <c r="A167" s="91" t="s">
         <v>446</v>
       </c>
@@ -23925,7 +23938,7 @@
         <v>219909</v>
       </c>
     </row>
-    <row r="168" spans="1:19">
+    <row r="168" spans="1:19" hidden="1">
       <c r="A168" s="97" t="s">
         <v>50</v>
       </c>
@@ -23980,7 +23993,7 @@
       </c>
       <c r="S168" s="91"/>
     </row>
-    <row r="169" spans="1:19">
+    <row r="169" spans="1:19" hidden="1">
       <c r="A169" s="157"/>
       <c r="B169" s="97"/>
       <c r="C169" s="89"/>
@@ -24001,7 +24014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:19">
+    <row r="170" spans="1:19" hidden="1">
       <c r="A170" s="157" t="s">
         <v>73</v>
       </c>
@@ -24055,7 +24068,7 @@
       </c>
       <c r="S170" s="91"/>
     </row>
-    <row r="171" spans="1:19">
+    <row r="171" spans="1:19" hidden="1">
       <c r="A171" s="105" t="s">
         <v>632</v>
       </c>
@@ -24104,7 +24117,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="172" spans="1:19">
+    <row r="172" spans="1:19" hidden="1">
       <c r="A172" s="91" t="s">
         <v>44</v>
       </c>
@@ -24162,13 +24175,13 @@
       </c>
       <c r="S172" s="40"/>
     </row>
-    <row r="173" spans="1:19">
+    <row r="173" spans="1:19" hidden="1">
       <c r="R173" s="93">
         <f t="shared" si="47"/>
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:19">
+    <row r="174" spans="1:19" hidden="1">
       <c r="A174" s="157"/>
       <c r="B174" s="97" t="s">
         <v>74</v>
@@ -24214,7 +24227,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="175" spans="1:19">
+    <row r="175" spans="1:19" hidden="1">
       <c r="A175" s="157"/>
       <c r="B175" s="97" t="s">
         <v>74</v>
@@ -24259,7 +24272,13 @@
       <c r="S175" s="91"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:S175" xr:uid="{5351C4FA-754E-4B23-BAD5-F50DA5EFAFB9}"/>
+  <autoFilter ref="A2:S175" xr:uid="{5351C4FA-754E-4B23-BAD5-F50DA5EFAFB9}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="4500095281"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="J1:J1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
@@ -33547,6 +33566,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008963B058EDD76E48B607691D37AC8497" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61d40ef7909dee5fad18dd73fcedc1cc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="251f237a-9322-4f80-991a-0286b9a96938" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fc473bdaa30bd3b96b900ea75e12c080" ns2:_="">
     <xsd:import namespace="251f237a-9322-4f80-991a-0286b9a96938"/>
@@ -33684,22 +33718,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{221000F8-CAE0-40B1-8AA0-FC8E2527B63F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7BCD85-DEC7-4080-A477-0C2765ACACC0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B15BA414-51C3-41E6-9EA2-0A58ECA893B2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33715,21 +33751,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7BCD85-DEC7-4080-A477-0C2765ACACC0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{221000F8-CAE0-40B1-8AA0-FC8E2527B63F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>